<commit_message>
【提交类型】：配件第一批需求 (1)128  (2)198 【功能描述】： 【问题说明】： 【修改内容】： 前端： bhmc-dcs-dev\bhmc-dcs-web\src\main\webapp\WEB-INF\jsp\par\pmm\itemMaster\selectItemMasterMain.jsp bhmc-dms-dev/bhmc-dms-web/src/main/webapp/WEB-INF/jsp/par/pmm/venderMaster/selectVenderMasterMain.jsp bhmc-dms-dev\bhmc-dms-web\src\main\webapp\WEB-INF\resources\excelDownloadTemplate\jexcel\PartItemMasterTarget_Tpl.xls bhmc-dms-dev\bhmc-dms-web\src\main\webapp\WEB-INF\resources\excelDownloadTemplate\poi\PartItemMasterTarget_Tpl.xlsx
后端：
bhmc-dms-dev\bhmc-dms-support\src\main\java\chn\bhmc\dms\par\pmm\vo\ItemMasterExcelDownVO.java
bhmc-dms-dev\bhmc-dms-support\src\main\resources\sqlmap\oracle\chn\bhmc\dms\par\pmm\ItemMasterDAO_SqlMap.xml
bhmc-dms-dev\bhmc-dms-support\src\main\java\chn\bhmc\dms\par\pmm\service\impl\ItemMasterServiceImpl.java
</commit_message>
<xml_diff>
--- a/bhmc-dms-dev/bhmc-dms-web/src/main/webapp/WEB-INF/resources/excelDownloadTemplate/poi/PartItemMasterTarget_Tpl.xlsx
+++ b/bhmc-dms-dev/bhmc-dms-web/src/main/webapp/WEB-INF/resources/excelDownloadTemplate/poi/PartItemMasterTarget_Tpl.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\6500955\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\source\bhmc_0511_fromGitWangchen\source\bhmc-dms-dev\bhmc-dms-web\src\main\webapp\WEB-INF\resources\excelDownloadTemplate\poi\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F3AA9D-DA3D-4171-B313-C7A94EFB2115}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1 " sheetId="2" r:id="rId1"/>
@@ -25,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>vmware</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -50,11 +51,11 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:area(lastCell="L4")</t>
+jx:area(lastCell="N4")</t>
         </r>
       </text>
     </comment>
-    <comment ref="A4" authorId="0" shapeId="0">
+    <comment ref="A4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -74,7 +75,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-jx:each(items="items" var="item" lastCell="L4")</t>
+jx:each(items="items" var="item" lastCell="N4")</t>
         </r>
       </text>
     </comment>
@@ -83,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="40">
   <si>
     <t>${item.newRplcParCmptYn}</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -138,7 +139,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -150,7 +151,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -162,7 +163,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -174,7 +175,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -186,7 +187,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -198,7 +199,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -213,7 +214,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -225,7 +226,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -237,7 +238,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -249,7 +250,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -267,7 +268,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -282,7 +283,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -294,7 +295,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -306,7 +307,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -321,7 +322,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -333,7 +334,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -345,7 +346,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -357,7 +358,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -375,7 +376,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -387,7 +388,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -405,7 +406,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -417,7 +418,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -432,7 +433,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -444,7 +445,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="136"/>
         <scheme val="minor"/>
@@ -462,7 +463,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -474,7 +475,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -496,7 +497,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -514,7 +515,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -526,7 +527,7 @@
         <b/>
         <sz val="11"/>
         <color theme="0"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -575,7 +576,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="3"/>
         <charset val="134"/>
         <scheme val="minor"/>
@@ -586,7 +587,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="맑은 고딕"/>
+        <rFont val="宋体"/>
         <family val="2"/>
         <charset val="129"/>
         <scheme val="minor"/>
@@ -597,18 +598,42 @@
   </si>
   <si>
     <t>00030689</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>供应商类型</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>供应商代码</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BMP</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>A10AA001</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${item.bpTpNm}</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>${item.bpCd}</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -616,14 +641,14 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -638,7 +663,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -647,7 +672,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="129"/>
       <scheme val="minor"/>
@@ -656,7 +681,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -665,7 +690,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="136"/>
       <scheme val="minor"/>
@@ -686,7 +711,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="맑은 고딕"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -738,7 +763,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,10 +788,25 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="표준" xfId="0" builtinId="0"/>
-    <cellStyle name="표준 2" xfId="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="표준 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1048,14 +1088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" style="1" customWidth="1"/>
@@ -1064,14 +1104,16 @@
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="23.25" style="11" customWidth="1"/>
+    <col min="10" max="10" width="24.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="36" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1082,12 +1124,14 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="I1" s="9"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1112,20 +1156,26 @@
       <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -1150,16 +1200,22 @@
       <c r="H4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="K4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1172,14 +1228,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="2" width="15" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.125" style="1" customWidth="1"/>
@@ -1188,14 +1244,16 @@
     <col min="6" max="6" width="17" style="1" customWidth="1"/>
     <col min="7" max="7" width="18.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19.625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20.75" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.125" style="1" customWidth="1"/>
-    <col min="12" max="12" width="24" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9" style="1"/>
+    <col min="9" max="9" width="23.25" style="11" customWidth="1"/>
+    <col min="10" max="10" width="24.125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="19.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="20.75" style="1" customWidth="1"/>
+    <col min="13" max="13" width="23.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="1" customWidth="1"/>
+    <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" ht="36" customHeight="1">
       <c r="A1" s="4" t="s">
         <v>24</v>
       </c>
@@ -1206,12 +1264,14 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="I1" s="9"/>
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14">
       <c r="A3" s="5" t="s">
         <v>23</v>
       </c>
@@ -1236,20 +1296,26 @@
       <c r="H3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="M3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="N3" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14">
       <c r="A4" s="3" t="s">
         <v>33</v>
       </c>
@@ -1274,12 +1340,18 @@
       <c r="H4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="I4" s="2"/>
+      <c r="I4" s="12" t="s">
+        <v>36</v>
+      </c>
       <c r="J4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>